<commit_message>
Added final details to lecture 1
</commit_message>
<xml_diff>
--- a/Data Wrangling.xlsx
+++ b/Data Wrangling.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JR29\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jctep\OneDrive\Documents\GitHub\data-wrangling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAABB167-F154-4A92-8595-83F26B15F476}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C0500A89-BA12-4956-B98B-3B6354A94363}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10110" xr2:uid="{A79E27F1-B037-4A7E-A0C5-DF3A90E9C58B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10116" xr2:uid="{A79E27F1-B037-4A7E-A0C5-DF3A90E9C58B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017" calcCompleted="0"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -196,7 +196,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,6 +215,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="25">
     <border>
@@ -514,7 +520,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -523,175 +529,205 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1008,573 +1044,577 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2066B0E4-E969-43F8-AEA9-08A8FF2D1A6B}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:B13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="10" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="60" customFormat="1" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:5" s="32" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="57" t="s">
+      <c r="D1" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="59" t="s">
+      <c r="E1" s="31" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="14">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="61">
         <v>1</v>
       </c>
-      <c r="B2" s="34">
+      <c r="B2" s="60">
         <v>1</v>
       </c>
-      <c r="C2" s="45" t="s">
+      <c r="C2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="35">
+    <row r="3" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="62"/>
+      <c r="B3" s="67">
         <v>2</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="33" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="17"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="7"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="26">
+    <row r="4" spans="1:5" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="63"/>
+      <c r="B4" s="68"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="34"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="64">
         <v>2</v>
       </c>
-      <c r="B5" s="37">
+      <c r="B5" s="69">
         <v>3</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="51" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="38"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="12" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="62"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="38"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="12" t="s">
+      <c r="E6" s="52"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="62"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="29"/>
-      <c r="B8" s="39">
+      <c r="E7" s="52"/>
+    </row>
+    <row r="8" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="65"/>
+      <c r="B8" s="70">
         <v>4</v>
       </c>
-      <c r="C8" s="50" t="s">
+      <c r="C8" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="15" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="14">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="39">
         <v>3</v>
       </c>
-      <c r="B9" s="40">
+      <c r="B9" s="42">
         <v>5</v>
       </c>
-      <c r="C9" s="45" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="10" t="s">
+      <c r="C9" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="34" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="51" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="13" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="40"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="7"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="51" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="13" t="s">
+      <c r="E10" s="34"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="40"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="7"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="51" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="13" t="s">
+      <c r="E11" s="34"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="40"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="7"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="51" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="13" t="s">
+      <c r="E12" s="34"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="40"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="17"/>
-      <c r="B14" s="41">
+      <c r="E13" s="35"/>
+    </row>
+    <row r="14" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="41"/>
+      <c r="B14" s="19">
         <v>6</v>
       </c>
-      <c r="C14" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="20" t="s">
+      <c r="C14" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E14" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="26">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="44">
         <v>4</v>
       </c>
-      <c r="B15" s="37">
+      <c r="B15" s="47">
         <v>7</v>
       </c>
-      <c r="C15" s="53" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="27" t="s">
+      <c r="C15" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="32" t="s">
+      <c r="E15" s="36" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
-      <c r="B16" s="38"/>
-      <c r="C16" s="54" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="12" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="45"/>
+      <c r="B16" s="48"/>
+      <c r="C16" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="8"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
-      <c r="B17" s="38"/>
-      <c r="C17" s="54" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="12" t="s">
+      <c r="E16" s="37"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="45"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="9"/>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="29"/>
-      <c r="B18" s="39">
+      <c r="E17" s="38"/>
+    </row>
+    <row r="18" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="46"/>
+      <c r="B18" s="18">
         <v>8</v>
       </c>
-      <c r="C18" s="50" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="30" t="s">
+      <c r="C18" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="31" t="s">
+      <c r="E18" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="18">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="50">
         <v>5</v>
       </c>
-      <c r="B19" s="42">
+      <c r="B19" s="49">
         <v>9</v>
       </c>
-      <c r="C19" s="45" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="10" t="s">
+      <c r="C19" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="34" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
-      <c r="B20" s="42"/>
-      <c r="C20" s="51" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="13" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="50"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="7"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
-      <c r="B21" s="40"/>
-      <c r="C21" s="51" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" s="13" t="s">
+      <c r="E20" s="34"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="50"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="5"/>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="18"/>
-      <c r="B22" s="41">
+      <c r="E21" s="35"/>
+    </row>
+    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="50"/>
+      <c r="B22" s="19">
         <v>10</v>
       </c>
-      <c r="C22" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="20" t="s">
+      <c r="C22" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="22" t="s">
+      <c r="E22" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="26">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="44">
         <v>6</v>
       </c>
-      <c r="B23" s="43">
+      <c r="B23" s="20">
         <v>11</v>
       </c>
-      <c r="C23" s="53" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="27" t="s">
+      <c r="C23" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="E23" s="33" t="s">
+      <c r="E23" s="16" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="29"/>
-      <c r="B24" s="39">
+    <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="46"/>
+      <c r="B24" s="18">
         <v>12</v>
       </c>
-      <c r="C24" s="50" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" s="30" t="s">
+      <c r="C24" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E24" s="31" t="s">
+      <c r="E24" s="15" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="14">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="39">
         <v>7</v>
       </c>
-      <c r="B25" s="34">
+      <c r="B25" s="17">
         <v>13</v>
       </c>
-      <c r="C25" s="45" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="10" t="s">
+      <c r="C25" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="17"/>
-      <c r="B26" s="41">
+    <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="41"/>
+      <c r="B26" s="19">
         <v>14</v>
       </c>
-      <c r="C26" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="20" t="s">
+      <c r="C26" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E26" s="22" t="s">
+      <c r="E26" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="26">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="44">
         <v>8</v>
       </c>
-      <c r="B27" s="43">
+      <c r="B27" s="20">
         <v>15</v>
       </c>
-      <c r="C27" s="53" t="s">
+      <c r="C27" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="D27" s="27" t="s">
+      <c r="D27" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E27" s="33" t="s">
+      <c r="E27" s="16" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="29"/>
-      <c r="B28" s="39">
-        <v>16</v>
-      </c>
-      <c r="C28" s="50" t="s">
+    <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="46"/>
+      <c r="B28" s="18">
+        <v>16</v>
+      </c>
+      <c r="C28" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="30" t="s">
+      <c r="D28" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E28" s="31" t="s">
+      <c r="E28" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="14">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="39">
         <v>9</v>
       </c>
-      <c r="B29" s="34">
+      <c r="B29" s="17">
         <v>17</v>
       </c>
-      <c r="C29" s="45" t="s">
+      <c r="C29" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="17"/>
-      <c r="B30" s="41">
+    <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="41"/>
+      <c r="B30" s="19">
         <v>18</v>
       </c>
-      <c r="C30" s="52" t="s">
+      <c r="C30" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D30" s="20" t="s">
+      <c r="D30" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E30" s="22" t="s">
+      <c r="E30" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="26">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="44">
         <v>10</v>
       </c>
-      <c r="B31" s="43">
+      <c r="B31" s="20">
         <v>19</v>
       </c>
-      <c r="C31" s="53" t="s">
+      <c r="C31" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="D31" s="27" t="s">
+      <c r="D31" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E31" s="33" t="s">
+      <c r="E31" s="16" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="29"/>
-      <c r="B32" s="39">
+    <row r="32" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="46"/>
+      <c r="B32" s="18">
         <v>20</v>
       </c>
-      <c r="C32" s="50" t="s">
+      <c r="C32" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D32" s="30" t="s">
+      <c r="D32" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E32" s="31" t="s">
+      <c r="E32" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="14">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="39">
         <v>11</v>
       </c>
-      <c r="B33" s="40">
+      <c r="B33" s="42">
         <v>21</v>
       </c>
-      <c r="C33" s="55" t="s">
+      <c r="C33" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="D33" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="E33" s="34" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="15"/>
-      <c r="B34" s="35"/>
-      <c r="C34" s="46"/>
-      <c r="D34" s="11" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="40"/>
+      <c r="B34" s="43"/>
+      <c r="C34" s="57"/>
+      <c r="D34" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="E34" s="7"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="15"/>
-      <c r="B35" s="35"/>
-      <c r="C35" s="46"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="5"/>
-    </row>
-    <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="17"/>
-      <c r="B36" s="41">
+      <c r="E34" s="34"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="40"/>
+      <c r="B35" s="43"/>
+      <c r="C35" s="57"/>
+      <c r="D35" s="53"/>
+      <c r="E35" s="35"/>
+    </row>
+    <row r="36" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="41"/>
+      <c r="B36" s="19">
         <v>22</v>
       </c>
-      <c r="C36" s="52" t="s">
+      <c r="C36" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="D36" s="20" t="s">
+      <c r="D36" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E36" s="22" t="s">
+      <c r="E36" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="26">
+    <row r="37" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="44">
         <v>12</v>
       </c>
-      <c r="B37" s="43">
+      <c r="B37" s="66">
         <v>23</v>
       </c>
-      <c r="C37" s="53" t="s">
+      <c r="C37" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D37" s="27" t="s">
+      <c r="D37" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E37" s="33" t="s">
+      <c r="E37" s="16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="29"/>
-      <c r="B38" s="39">
+    <row r="38" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="46"/>
+      <c r="B38" s="18">
         <v>24</v>
       </c>
-      <c r="C38" s="50" t="s">
+      <c r="C38" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D38" s="30" t="s">
+      <c r="D38" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E38" s="31" t="s">
+      <c r="E38" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="23"/>
-      <c r="B39" s="44" t="s">
+    <row r="39" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="10"/>
+      <c r="B39" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C39" s="56" t="s">
+      <c r="C39" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="D39" s="24" t="s">
+      <c r="D39" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E39" s="25"/>
+      <c r="E39" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="E33:E35"/>
-    <mergeCell ref="E9:E13"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="B9:B13"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="C33:C35"/>
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="A19:A22"/>
@@ -1582,18 +1622,16 @@
     <mergeCell ref="A33:A36"/>
     <mergeCell ref="B33:B35"/>
     <mergeCell ref="D34:D35"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="B9:B13"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E33:E35"/>
+    <mergeCell ref="E9:E13"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="E19:E21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>